<commit_message>
🔧 update excel api case.
</commit_message>
<xml_diff>
--- a/api_case/api_case.xlsx
+++ b/api_case/api_case.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29868" windowHeight="13380"/>
+    <workbookView windowWidth="19835" windowHeight="10704"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>简单</t>
     </r>
     <r>
@@ -111,7 +117,7 @@
 }</t>
   </si>
   <si>
-    <t>["X-Amzn-Trace-Id"]</t>
+    <t>["X-Amzn-Trace-Id","origin"]</t>
   </si>
   <si>
     <r>
@@ -798,12 +804,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -930,7 +951,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -942,34 +963,34 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1054,7 +1075,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1064,22 +1085,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1395,20 +1425,20 @@
   <sheetPr/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="24.3333333333333" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.1111111111111" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.8888888888889" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.2222222222222" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.22222222222222" style="2" customWidth="1"/>
     <col min="4" max="4" width="32.2222222222222" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.7777777777778" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8" style="2" customWidth="1"/>
     <col min="6" max="6" width="23.3333333333333" style="2" customWidth="1"/>
     <col min="7" max="7" width="43" style="2" customWidth="1"/>
-    <col min="8" max="8" width="21.7777777777778" style="2" customWidth="1"/>
+    <col min="8" max="8" width="25.2222222222222" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="15.6" spans="1:8">
@@ -1437,7 +1467,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" ht="207" spans="1:8">
+    <row r="2" ht="126" customHeight="1" spans="1:8">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -1463,7 +1493,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" ht="289.8" spans="1:8">
+    <row r="3" ht="130" customHeight="1" spans="1:8">
       <c r="A3" s="6" t="s">
         <v>16</v>
       </c>
@@ -1489,7 +1519,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" ht="303.6" spans="1:8">
+    <row r="4" ht="173" customHeight="1" spans="1:8">
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
@@ -1542,25 +1572,25 @@
       </c>
     </row>
     <row r="6" ht="303.6" spans="1:8">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="11" t="s">
         <v>34</v>
       </c>
       <c r="H6" s="6" t="s">

</xml_diff>

<commit_message>
:wrench: update api_excel case.
</commit_message>
<xml_diff>
--- a/api_case/api_case.xlsx
+++ b/api_case/api_case.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19835" windowHeight="10704"/>
+    <workbookView windowHeight="17691"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>name</t>
   </si>
@@ -199,6 +199,9 @@
   "origin": "14.155.89.115",
   "url": "http://www.httpbin.org/post"
 }</t>
+  </si>
+  <si>
+    <t>["X-Amzn-Trace-Id","origin","User-Agent"]</t>
   </si>
   <si>
     <r>
@@ -1425,23 +1428,23 @@
   <sheetPr/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.1" outlineLevelRow="5" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="24.3333333333333" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.2222222222222" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.22222222222222" style="2" customWidth="1"/>
-    <col min="4" max="4" width="32.2222222222222" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.2252252252252" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.22522522522523" style="2" customWidth="1"/>
+    <col min="4" max="4" width="32.2252252252252" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.5045045045045" style="2" customWidth="1"/>
     <col min="6" max="6" width="23.3333333333333" style="2" customWidth="1"/>
     <col min="7" max="7" width="43" style="2" customWidth="1"/>
-    <col min="8" max="8" width="25.2222222222222" style="2" customWidth="1"/>
+    <col min="8" max="8" width="25.2252252252252" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="15.6" spans="1:8">
+    <row r="1" s="1" customFormat="1" ht="15" spans="1:8">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1516,12 +1519,12 @@
         <v>21</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" ht="173" customHeight="1" spans="1:8">
       <c r="A4" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>17</v>
@@ -1536,24 +1539,24 @@
         <v>12</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="5" ht="317.4" spans="1:8">
+    <row r="5" ht="324.45" spans="1:8">
       <c r="A5" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>19</v>
@@ -1562,24 +1565,24 @@
         <v>12</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="6" ht="303.6" spans="1:8">
+    <row r="6" ht="310.3" spans="1:8">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>19</v>
@@ -1588,13 +1591,13 @@
         <v>12</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>